<commit_message>
updated for response variations
</commit_message>
<xml_diff>
--- a/data/responses_data.xlsx
+++ b/data/responses_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RASA CHATBOT\marlabs_chatbot\rasa_marlabs_chatbot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1539A801-56F4-4738-9AD8-21429748BC5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F69931F2-0CC9-43E5-A306-3F9E3536F8F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>S.N.</t>
   </si>
@@ -67,9 +67,6 @@
   <si>
     <t>I have an enquiry pertaining to:
 Business | Media | Careers | Other [links]</t>
-  </si>
-  <si>
-    <t>welcome message</t>
   </si>
   <si>
     <t>utter_greet</t>
@@ -99,9 +96,6 @@
     </r>
   </si>
   <si>
-    <t>I want to know more about Marlabs:/about_marlabs, What do you do?:/what_do_you_do, I’m interested in a career with Marlabs:/marlabs_career, I want to talk to a digital advisor:/talk_to_advisor, Read your latest publications:/latest_publications</t>
-  </si>
-  <si>
     <t>RESPONSE NAME</t>
   </si>
   <si>
@@ -141,13 +135,48 @@
     <t>If you love solving complex challenges through technology and working with some of the smartest minds, we would love to meet you! Head over to our 
 &lt;a href="https://career.marlabs.com"&gt;careers&lt;/a&gt; section for a list of current job openings.</t>
   </si>
+  <si>
+    <t>Goodbye message</t>
+  </si>
+  <si>
+    <t>Welcome message</t>
+  </si>
+  <si>
+    <t>utter_goodbye</t>
+  </si>
+  <si>
+    <t>Goodbye! It was nice talking to you.;
+Bye for now. Have a great day!;
+Thank you for chatting with me. Bye!;
+Goodbye! If you have any more questions, don't hesitate to ask.;
+Bye, have a great day.</t>
+  </si>
+  <si>
+    <t>I want to know more about Marlabs:/about_marlabs,
+What do you do?:/what_do_you_do,
+I’m interested in a career with Marlabs:/marlabs_career,
+I want to talk to a digital advisor:/talk_to_advisor,
+Read your latest publications:/latest_publications</t>
+  </si>
+  <si>
+    <t>utter_type_query_below</t>
+  </si>
+  <si>
+    <t>Please type your query below.</t>
+  </si>
+  <si>
+    <t>utter_can_i_help_more</t>
+  </si>
+  <si>
+    <t>Can i help you with anything more?</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0;[Red]0"/>
+    <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -190,12 +219,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF4472C4"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -218,46 +245,37 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -266,7 +284,77 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="12">
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0;[Red]0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -277,6 +365,30 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7A373A29-A40A-49D7-B22B-66B17608779F}" name="Responses" displayName="Responses" ref="A1:F10">
+  <autoFilter ref="A1:F10" xr:uid="{7A373A29-A40A-49D7-B22B-66B17608779F}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{A9B0D077-0D3E-4D57-B08D-A540E077092C}" name="S.N." totalsRowLabel="Total" dataDxfId="2" totalsRowDxfId="4">
+      <calculatedColumnFormula>ROWS($A$2:Responses[[#This Row],[RESPONSE NAME]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{FE327F13-77D6-4B47-ABFC-282C6A5C67E4}" name="QUESTION" dataDxfId="0" totalsRowDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{9AD1DB3D-3C9D-47A1-88B8-C69D9A2237E5}" name="RESPONSE NAME" dataDxfId="1" totalsRowDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{390E63D5-5C66-4753-87DD-5AC253A711BE}" name="TEXT" dataDxfId="3" totalsRowDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{85B51E21-54C3-4CE9-ACBD-D991C12A4CFA}" name="BUTTON" dataDxfId="11" totalsRowDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{28CD2182-8E6C-4AAE-9965-7BEC3002A73B}" name="URL" totalsRowFunction="count" dataDxfId="10" totalsRowDxfId="9"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -542,138 +654,179 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.42578125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" style="6" customWidth="1"/>
-    <col min="4" max="4" width="54.28515625" style="7" customWidth="1"/>
-    <col min="5" max="5" width="54.85546875" style="12" customWidth="1"/>
-    <col min="6" max="8" width="9.140625" style="8"/>
-    <col min="9" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="8.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="31" style="8" customWidth="1"/>
+    <col min="4" max="4" width="65.42578125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="54.85546875" style="6" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" s="9">
+        <f>ROWS($A$2:Responses[[#This Row],[RESPONSE NAME]])</f>
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" s="9">
+        <f>ROWS($A$2:Responses[[#This Row],[RESPONSE NAME]])</f>
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="9">
+        <f>ROWS($A$2:Responses[[#This Row],[RESPONSE NAME]])</f>
+        <v>3</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="9">
+        <f>ROWS($A$2:Responses[[#This Row],[RESPONSE NAME]])</f>
+        <v>4</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
+        <f>ROWS($A$2:Responses[[#This Row],[RESPONSE NAME]])</f>
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="7" t="s">
+      <c r="D6" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="285" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
+        <f>ROWS($A$2:Responses[[#This Row],[RESPONSE NAME]])</f>
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
+        <f>ROWS($A$2:Responses[[#This Row],[RESPONSE NAME]])</f>
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" s="9">
+        <f>ROWS($A$2:Responses[[#This Row],[RESPONSE NAME]])</f>
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <f>ROWS($A$2:Responses[[#This Row],[RESPONSE NAME]])</f>
+        <v>9</v>
+      </c>
+      <c r="B10" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>2</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="165" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="9" t="s">
+      <c r="C10" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D10" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="285" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
-        <v>4</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
-        <v>5</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="150" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
-        <v>6</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D9" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
retrained model and added nlu_fallback intent
</commit_message>
<xml_diff>
--- a/data/responses_data.xlsx
+++ b/data/responses_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RASA CHATBOT\marlabs_chatbot\rasa_marlabs_chatbot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F69931F2-0CC9-43E5-A306-3F9E3536F8F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BF6962C-16BB-4FC0-A032-7D548F02CB82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>S.N.</t>
   </si>
@@ -169,6 +169,12 @@
   </si>
   <si>
     <t>Can i help you with anything more?</t>
+  </si>
+  <si>
+    <t>I'm sorry, I didn't quite understand that. could you rephrase your query?</t>
+  </si>
+  <si>
+    <t>utter_please_rephrase</t>
   </si>
 </sst>
 </file>
@@ -368,8 +374,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7A373A29-A40A-49D7-B22B-66B17608779F}" name="Responses" displayName="Responses" ref="A1:F10">
-  <autoFilter ref="A1:F10" xr:uid="{7A373A29-A40A-49D7-B22B-66B17608779F}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7A373A29-A40A-49D7-B22B-66B17608779F}" name="Responses" displayName="Responses" ref="A1:F11">
+  <autoFilter ref="A1:F11" xr:uid="{7A373A29-A40A-49D7-B22B-66B17608779F}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -654,10 +660,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -735,7 +741,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <f>ROWS($A$2:Responses[[#This Row],[RESPONSE NAME]])</f>
         <v>4</v>
@@ -747,78 +753,90 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <f>ROWS($A$2:Responses[[#This Row],[RESPONSE NAME]])</f>
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
+        <f>ROWS($A$2:Responses[[#This Row],[RESPONSE NAME]])</f>
         <v>6</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="B7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D7" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="285" x14ac:dyDescent="0.25">
-      <c r="A7" s="9">
-        <f>ROWS($A$2:Responses[[#This Row],[RESPONSE NAME]])</f>
-        <v>6</v>
-      </c>
-      <c r="B7" s="3" t="s">
+    <row r="8" spans="1:6" ht="285" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
+        <f>ROWS($A$2:Responses[[#This Row],[RESPONSE NAME]])</f>
         <v>7</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="B8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D8" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="9">
-        <f>ROWS($A$2:Responses[[#This Row],[RESPONSE NAME]])</f>
-        <v>7</v>
-      </c>
-      <c r="B8" s="3" t="s">
+    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="9">
+        <f>ROWS($A$2:Responses[[#This Row],[RESPONSE NAME]])</f>
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C9" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D9" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A9" s="9">
-        <f>ROWS($A$2:Responses[[#This Row],[RESPONSE NAME]])</f>
+    <row r="10" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <f>ROWS($A$2:Responses[[#This Row],[RESPONSE NAME]])</f>
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="5" t="s">
+      <c r="C10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D10" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="150" x14ac:dyDescent="0.25">
-      <c r="A10" s="9">
-        <f>ROWS($A$2:Responses[[#This Row],[RESPONSE NAME]])</f>
-        <v>9</v>
-      </c>
-      <c r="B10" s="10" t="s">
+    <row r="11" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+      <c r="A11" s="9">
+        <f>ROWS($A$2:Responses[[#This Row],[RESPONSE NAME]])</f>
+        <v>10</v>
+      </c>
+      <c r="B11" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C11" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
new changes with added test cases
</commit_message>
<xml_diff>
--- a/data/responses_data.xlsx
+++ b/data/responses_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RASA CHATBOT\marlabs_chatbot\rasa_marlabs_chatbot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25D2D268-BBE9-4B4D-B264-8105862D836B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F41D8795-AE9F-4E2A-AC39-212BE6728246}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="responses" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -149,10 +148,6 @@
     <t>Automation;https://www.marlabs.com/intelligent-automation/|Customer experience;https://www.marlabs.com/human-experience/|Cybersecurity;https://www.marlabs.com/cybersecurity/|AI, data &amp; analytics;https://www.marlabs.com/data-analytics-ai/</t>
   </si>
   <si>
-    <t>Read more on the latest in the world of business and technology: \n
-&lt;a href="https://www.marlabs.com/digital-victories/"&gt;Case studies&lt;/a&gt; | &lt;a href="https://www.marlabs.com/now-and-next/"&gt;Whitepapers&lt;/a&gt; | &lt;a href="https://www.marlabs.com/now-and-next/"&gt;Podcasts&lt;/a&gt; | &lt;a href="https://www.marlabs.com/now-and-next/"&gt;Videos&lt;/a&gt;</t>
-  </si>
-  <si>
     <t>Marlabs helps leading companies around the world make operations sleeker, keep customers closer, transform data into decisions, de-risk cyberspace, boost legacy systems, and capture novel opportunities and digital-led revenues.\n
 We are headquartered in New Jersey, with offices in the US, Germany, Canada, and India. Our 3,000+ global workforce includes highly experienced technology, platform, and industry specialists from the world’s leading technical universities.</t>
   </si>
@@ -189,6 +184,10 @@
   </si>
   <si>
     <t>Sure, feel free to browse around. Goodbye for now.</t>
+  </si>
+  <si>
+    <t>Read more on the latest in the world of business and technology: \n
+&lt;a href="https://www.marlabs.com/digital-victories/" target="_blank"&gt;Case studies&lt;/a&gt; | &lt;a href="https://www.marlabs.com/now-and-next/" target="_blank"&gt;Whitepapers&lt;/a&gt; | &lt;a href="https://www.marlabs.com/now-and-next/" target="_blank"&gt;Podcasts&lt;/a&gt; | &lt;a href="https://www.marlabs.com/now-and-next/" target="_blank"&gt;Videos&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
@@ -676,8 +675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -723,7 +722,7 @@
         <v>9</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -732,19 +731,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>38</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>21</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -759,7 +758,7 @@
         <v>20</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -783,7 +782,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>22</v>
@@ -798,7 +797,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>27</v>
@@ -819,7 +818,7 @@
         <v>13</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="135" x14ac:dyDescent="0.25">
@@ -834,7 +833,7 @@
         <v>16</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>28</v>
@@ -852,10 +851,10 @@
         <v>12</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -873,7 +872,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <f>ROWS($A$2:Responses[[#This Row],[RESPONSE NAME]])</f>
         <v>11</v>
@@ -885,7 +884,7 @@
         <v>15</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>